<commit_message>
fix cross ref, update timetable
</commit_message>
<xml_diff>
--- a/specifics/DS2-22-WiSe-Modulverlauf.xlsx
+++ b/specifics/DS2-22-WiSe-Modulverlauf.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastiansaueruser/github-repos/datascience2/specifics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastiansaueruser/github-repos/datascience-text/specifics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF137B07-FB3F-6D4C-B945-54709308B0D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EF6009-E8FB-E541-9FBD-DB605B190FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16900" xr2:uid="{B4BA407F-7EF6-F641-926D-2394B79BC202}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Nr</t>
   </si>
@@ -130,10 +130,10 @@
     <t>Quarto Blog</t>
   </si>
   <si>
-    <t>Coaching</t>
-  </si>
-  <si>
     <t>Die erste Unterrichtsstunde fällt auf den 6. Okt. 2023.</t>
+  </si>
+  <si>
+    <t>Am 3. November entfällt der Unterricht in diesem Modul.</t>
   </si>
 </sst>
 </file>
@@ -497,7 +497,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -532,7 +532,7 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -551,7 +551,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -562,7 +562,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -573,10 +573,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -584,7 +587,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -603,7 +606,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -614,7 +617,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -625,7 +628,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
@@ -636,7 +639,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
         <v>16</v>
@@ -647,7 +650,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
         <v>17</v>

</xml_diff>